<commit_message>
Updated Excel spreadsheet with new logic.
</commit_message>
<xml_diff>
--- a/PublicDebtChargesCalculator/public_debt_charges_calculator_worksheet.xlsx
+++ b/PublicDebtChargesCalculator/public_debt_charges_calculator_worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hoc-cdc.ca\AdminPrivate\FS06U\BergeE\Documents\Interest rate tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hoc-cdc.ca\AdminPrivate\FS06U\MatieC\Documents\EPC\Ready_Reckoner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244FE866-6DCD-49B5-9FF0-010F6B77E165}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FE243-AEC7-4E73-ADC9-7D6F6B9FD3D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
   <sheets>
     <sheet name="Pour utilisateur" sheetId="3" r:id="rId1"/>
@@ -68,15 +68,6 @@
     <t>Marginal effective interest rate</t>
   </si>
   <si>
-    <t>debt charges on primary balances</t>
-  </si>
-  <si>
-    <t>debt charges on cumulative primary balances</t>
-  </si>
-  <si>
-    <t>debt charges on debt charges</t>
-  </si>
-  <si>
     <t>OUTPUT</t>
   </si>
   <si>
@@ -143,26 +134,36 @@
     <t>Frais d'intérêt sur la balance primaire</t>
   </si>
   <si>
-    <t>Frais d'intérêt sur les balances primaires cumulés</t>
-  </si>
-  <si>
-    <t>Intérêts sur les intérêts</t>
-  </si>
-  <si>
     <t>Frais d'intérêt totaux</t>
   </si>
   <si>
     <t>Arrière-plan</t>
+  </si>
+  <si>
+    <t>Debt charges on primary balances</t>
+  </si>
+  <si>
+    <t>New borrowing</t>
+  </si>
+  <si>
+    <t>Stock of borrowing</t>
+  </si>
+  <si>
+    <t>Stock des obligations</t>
+  </si>
+  <si>
+    <t>Obligations supplémentaires</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -277,7 +278,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -307,6 +308,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -625,9 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59573D42-40D1-4AAE-B281-D9DA5023429D}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -637,7 +639,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1">
         <v>2019</v>
@@ -756,10 +758,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -800,10 +802,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -844,10 +846,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4">
         <f>C4-C5</f>
@@ -900,7 +902,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
@@ -918,10 +920,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="16">
         <f>'Non-modifiable'!C21</f>
@@ -974,10 +976,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C11" s="16">
         <f>'Non-modifiable'!C22</f>
@@ -1030,10 +1032,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C12" s="16">
         <f>'Non-modifiable'!C21+'Non-modifiable'!C6</f>
@@ -1086,10 +1088,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="20" t="e">
         <f>'Non-modifiable'!C21/'Non-modifiable'!C22</f>
@@ -1142,7 +1144,7 @@
     </row>
     <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -1168,9 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8F7545-787E-47D5-A81D-527FE013B894}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1392,11 +1392,11 @@
         <v>5</v>
       </c>
       <c r="C6" s="4">
-        <f>C4-C5</f>
+        <f t="shared" ref="C6:N6" si="1">C4-C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:N6" si="1">D4-D5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E6" s="4">
@@ -1442,7 +1442,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>5</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>5</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>5</v>
@@ -1628,10 +1628,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="20" t="e">
         <f>'Non-modifiable (EN)'!C21/'Non-modifiable (EN)'!C22</f>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" s="19"/>
     </row>
@@ -1705,9 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F899D073-8803-4D1C-833B-2BB3523900F5}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1717,7 +1715,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1">
         <v>2019</v>
@@ -1836,10 +1834,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4">
         <f>'Pour utilisateur'!C4</f>
@@ -1892,10 +1890,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4">
         <f>'Pour utilisateur'!C5</f>
@@ -1948,10 +1946,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4">
         <f>'Pour utilisateur'!C6</f>
@@ -2004,7 +2002,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2022,7 +2020,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="8">
@@ -2080,7 +2078,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="9">
@@ -2122,7 +2120,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="9">
@@ -2164,7 +2162,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="9">
@@ -2250,7 +2248,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="10">
@@ -2304,112 +2302,115 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="10">
-        <f>SUM($C16:C16)</f>
+        <f>-(C6+C16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <f>SUM($C16:D16)</f>
+        <f t="shared" ref="D17:N17" si="3">-(D6+D16)</f>
         <v>0</v>
       </c>
       <c r="E17" s="10">
-        <f>SUM($C16:E16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F17" s="10">
-        <f>SUM($C16:F16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G17" s="10">
-        <f>SUM($C16:G16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H17" s="10">
-        <f>SUM($C16:H16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17" s="10">
-        <f>SUM($C16:I16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J17" s="10">
-        <f>SUM($C16:J16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K17" s="10">
-        <f>SUM($C16:K16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L17" s="10">
-        <f>SUM($C16:L16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M17" s="10">
-        <f>SUM($C16:M16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N17" s="10">
-        <f>SUM($C16:N16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
+      <c r="C18" s="12">
+        <f>C17</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="12">
-        <f t="shared" ref="D18:N18" si="3">C17*(D13/100)</f>
+        <f>(1+D13/100)*C18+D17</f>
         <v>0</v>
       </c>
       <c r="E18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E18:N18" si="4">(1+E13/100)*D18+E17</f>
         <v>0</v>
       </c>
       <c r="F18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="14"/>
@@ -2427,109 +2428,109 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="16">
-        <f>SUM(C17:C18)</f>
+        <f>C16</f>
         <v>0</v>
       </c>
       <c r="D21" s="16">
-        <f t="shared" ref="D21:N21" si="4">SUM(D17:D18)</f>
+        <f>D16+D13/100*C22</f>
         <v>0</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E21:N21" si="5">E16+E13/100*D22</f>
         <v>0</v>
       </c>
       <c r="F21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="16">
-        <f>SUM($C6:C6)+C21</f>
+        <f>-C18</f>
         <v>0</v>
       </c>
       <c r="D22" s="16">
-        <f>SUM($C6:D6)+D21</f>
+        <f t="shared" ref="D22:N22" si="6">-D18</f>
         <v>0</v>
       </c>
       <c r="E22" s="16">
-        <f>SUM($C6:E6)+E21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F22" s="16">
-        <f>SUM($C6:F6)+F21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G22" s="16">
-        <f>SUM($C6:G6)+G21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H22" s="16">
-        <f>SUM($C6:H6)+H21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I22" s="16">
-        <f>SUM($C6:I6)+I21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J22" s="16">
-        <f>SUM($C6:J6)+J21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K22" s="16">
-        <f>SUM($C6:K6)+K21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L22" s="16">
-        <f>SUM($C6:L6)+L21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M22" s="16">
-        <f>SUM($C6:M6)+M21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N22" s="16">
-        <f>SUM($C6:N6)+N21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2540,18 +2541,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB77E90E-259F-4B12-BB0C-68506FD8C7E4}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2020</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2670,7 +2670,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -2838,12 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="U7">
-        <v>1.675</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2860,11 +2855,8 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-      <c r="U8">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -2905,11 +2897,8 @@
       <c r="N9" s="8">
         <v>0.82054017639366417</v>
       </c>
-      <c r="U9">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
@@ -2924,15 +2913,8 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
-      <c r="U10">
-        <v>1.95</v>
-      </c>
-      <c r="V10">
-        <f>AVERAGE(U7:U10)</f>
-        <v>1.7562500000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2973,11 +2955,8 @@
       <c r="N11" s="9">
         <v>2.7</v>
       </c>
-      <c r="U11">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -3018,11 +2997,8 @@
       <c r="N12" s="9">
         <v>3.75</v>
       </c>
-      <c r="U12">
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -3075,11 +3051,8 @@
         <f t="shared" si="1"/>
         <v>3.5615671852133475</v>
       </c>
-      <c r="U13">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3094,15 +3067,8 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
-      <c r="U14">
-        <v>2.7</v>
-      </c>
-      <c r="V14">
-        <f>AVERAGE(U11:U14)</f>
-        <v>2.5125000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3117,13 +3083,10 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
-      <c r="U15">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="10">
@@ -3174,124 +3137,118 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U16">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="10">
-        <f>SUM($C16:C16)</f>
+        <f>-(C6+C16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <f>SUM($C16:D16)</f>
+        <f t="shared" ref="D17:N17" si="3">-(D6+D16)</f>
         <v>0</v>
       </c>
       <c r="E17" s="10">
-        <f>SUM($C16:E16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F17" s="10">
-        <f>SUM($C16:F16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G17" s="10">
-        <f>SUM($C16:G16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H17" s="10">
-        <f>SUM($C16:H16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17" s="10">
-        <f>SUM($C16:I16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J17" s="10">
-        <f>SUM($C16:J16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K17" s="10">
-        <f>SUM($C16:K16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L17" s="10">
-        <f>SUM($C16:L16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M17" s="10">
-        <f>SUM($C16:M16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N17" s="10">
-        <f>SUM($C16:N16)</f>
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
+      <c r="C18" s="12">
+        <f>C17</f>
+        <v>0</v>
+      </c>
       <c r="D18" s="12">
-        <f t="shared" ref="D18:N18" si="3">C17*(D13/100)</f>
+        <f>(1+D13/100)*C18+D17</f>
         <v>0</v>
       </c>
       <c r="E18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E18:N18" si="4">(1+E13/100)*D18+E17</f>
         <v>0</v>
       </c>
       <c r="F18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M18" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N18" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="14"/>
@@ -3307,115 +3264,147 @@
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="16">
-        <f>SUM(C17:C18)</f>
+        <f>C16</f>
         <v>0</v>
       </c>
       <c r="D21" s="16">
-        <f t="shared" ref="D21:N21" si="4">SUM(D17:D18)</f>
+        <f>D16+D13/100*C22</f>
         <v>0</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E21:N21" si="5">E16+E13/100*D22</f>
         <v>0</v>
       </c>
       <c r="F21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M21" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N21" s="16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="16">
-        <f>SUM($C6:C6)+C21</f>
+        <f>-C18</f>
         <v>0</v>
       </c>
       <c r="D22" s="16">
-        <f>SUM($C6:D6)+D21</f>
+        <f t="shared" ref="D22:N22" si="6">-D18</f>
         <v>0</v>
       </c>
       <c r="E22" s="16">
-        <f>SUM($C6:E6)+E21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F22" s="16">
-        <f>SUM($C6:F6)+F21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G22" s="16">
-        <f>SUM($C6:G6)+G21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H22" s="16">
-        <f>SUM($C6:H6)+H21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I22" s="16">
-        <f>SUM($C6:I6)+I21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J22" s="16">
-        <f>SUM($C6:J6)+J21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K22" s="16">
-        <f>SUM($C6:K6)+K21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L22" s="16">
-        <f>SUM($C6:L6)+L21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M22" s="16">
-        <f>SUM($C6:M6)+M21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N22" s="16">
-        <f>SUM($C6:N6)+N21</f>
-        <v>0</v>
-      </c>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Limited range to 2019-2029.
</commit_message>
<xml_diff>
--- a/PublicDebtChargesCalculator/public_debt_charges_calculator_worksheet.xlsx
+++ b/PublicDebtChargesCalculator/public_debt_charges_calculator_worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hoc-cdc.ca\AdminPrivate\FS06U\MatieC\Documents\EPC\Ready_Reckoner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hoc-cdc.ca\AdminPrivate\FS06U\VanheR\Desktop\PublicDebtChargesCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23FE243-AEC7-4E73-ADC9-7D6F6B9FD3D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D1FA683-48CC-4248-B4A2-A3928EB8E951}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{983CEFC8-2B83-4647-BCB1-636BCC2A5490}"/>
   </bookViews>
   <sheets>
     <sheet name="Pour utilisateur" sheetId="3" r:id="rId1"/>
@@ -163,7 +163,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -309,7 +309,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -627,9 +627,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59573D42-40D1-4AAE-B281-D9DA5023429D}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -637,7 +639,7 @@
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -649,7 +651,7 @@
         <v>2020</v>
       </c>
       <c r="E1">
-        <f t="shared" ref="E1:N2" si="0">D1+1</f>
+        <f t="shared" ref="E1:L2" si="0">D1+1</f>
         <v>2021</v>
       </c>
       <c r="F1">
@@ -680,16 +682,8 @@
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="M1">
-        <f t="shared" si="0"/>
-        <v>2029</v>
-      </c>
-      <c r="N1">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2020</v>
       </c>
@@ -729,16 +723,8 @@
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-      <c r="N2">
-        <f t="shared" si="0"/>
-        <v>2031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,10 +739,8 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -793,14 +777,8 @@
       <c r="L4" s="4">
         <v>0</v>
       </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -837,14 +815,8 @@
       <c r="L5" s="4">
         <v>0</v>
       </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -856,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:N6" si="1">D4-D5</f>
+        <f t="shared" ref="D6:L6" si="1">D4-D5</f>
         <v>0</v>
       </c>
       <c r="E6" s="4">
@@ -891,16 +863,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
@@ -915,10 +879,8 @@
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
@@ -965,16 +927,8 @@
         <f>'Non-modifiable'!L21</f>
         <v>0</v>
       </c>
-      <c r="M10" s="16">
-        <f>'Non-modifiable'!M21</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="16">
-        <f>'Non-modifiable'!N21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
@@ -1021,16 +975,8 @@
         <f>'Non-modifiable'!L22</f>
         <v>0</v>
       </c>
-      <c r="M11" s="16">
-        <f>'Non-modifiable'!M22</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="16">
-        <f>'Non-modifiable'!N22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>21</v>
       </c>
@@ -1077,16 +1023,8 @@
         <f>'Non-modifiable'!L21+'Non-modifiable'!L6</f>
         <v>0</v>
       </c>
-      <c r="M12" s="16">
-        <f>'Non-modifiable'!M21+'Non-modifiable'!M6</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="16">
-        <f>'Non-modifiable'!N21+'Non-modifiable'!N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>27</v>
       </c>
@@ -1133,16 +1071,8 @@
         <f>'Non-modifiable'!L21/'Non-modifiable'!L22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="20" t="e">
-        <f>'Non-modifiable'!M21/'Non-modifiable'!M22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" s="20" t="e">
-        <f>'Non-modifiable'!N21/'Non-modifiable'!N22</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +1085,7 @@
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -1168,16 +1098,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8F7545-787E-47D5-A81D-527FE013B894}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1121,7 @@
         <v>2020</v>
       </c>
       <c r="E1">
-        <f t="shared" ref="E1:N2" si="0">D1+1</f>
+        <f t="shared" ref="E1:L2" si="0">D1+1</f>
         <v>2021</v>
       </c>
       <c r="F1">
@@ -1220,16 +1152,8 @@
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="M1">
-        <f t="shared" si="0"/>
-        <v>2029</v>
-      </c>
-      <c r="N1">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2020</v>
       </c>
@@ -1269,16 +1193,8 @@
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-      <c r="N2">
-        <f t="shared" si="0"/>
-        <v>2031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1293,10 +1209,8 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1333,14 +1247,8 @@
       <c r="L4" s="4">
         <v>0</v>
       </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1377,14 +1285,8 @@
       <c r="L5" s="4">
         <v>0</v>
       </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1294,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" ref="C6:N6" si="1">C4-C5</f>
+        <f t="shared" ref="C6:L6" si="1">C4-C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="4">
@@ -1431,16 +1333,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
@@ -1455,10 +1349,8 @@
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>12</v>
       </c>
@@ -1505,16 +1397,8 @@
         <f>'Non-modifiable (EN)'!L21</f>
         <v>0</v>
       </c>
-      <c r="M10" s="16">
-        <f>'Non-modifiable (EN)'!M21</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="16">
-        <f>'Non-modifiable (EN)'!N21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
@@ -1561,16 +1445,8 @@
         <f>'Non-modifiable (EN)'!L22</f>
         <v>0</v>
       </c>
-      <c r="M11" s="16">
-        <f>'Non-modifiable (EN)'!M22</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="16">
-        <f>'Non-modifiable (EN)'!N22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>23</v>
       </c>
@@ -1617,16 +1493,8 @@
         <f>'Non-modifiable (EN)'!L21+'Non-modifiable (EN)'!L6</f>
         <v>0</v>
       </c>
-      <c r="M12" s="16">
-        <f>'Non-modifiable (EN)'!M21+'Non-modifiable (EN)'!M6</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="16">
-        <f>'Non-modifiable (EN)'!N21+'Non-modifiable (EN)'!N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>25</v>
       </c>
@@ -1673,22 +1541,14 @@
         <f>'Non-modifiable (EN)'!L21/'Non-modifiable (EN)'!L22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="20" t="e">
-        <f>'Non-modifiable (EN)'!M21/'Non-modifiable (EN)'!M22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" s="20" t="e">
-        <f>'Non-modifiable (EN)'!N21/'Non-modifiable (EN)'!N22</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="19"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
     </row>
@@ -1703,9 +1563,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F899D073-8803-4D1C-833B-2BB3523900F5}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1713,7 +1575,7 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1725,7 +1587,7 @@
         <v>2020</v>
       </c>
       <c r="E1">
-        <f t="shared" ref="E1:N2" si="0">D1+1</f>
+        <f t="shared" ref="E1:L2" si="0">D1+1</f>
         <v>2021</v>
       </c>
       <c r="F1">
@@ -1756,16 +1618,8 @@
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="M1">
-        <f t="shared" si="0"/>
-        <v>2029</v>
-      </c>
-      <c r="N1">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2020</v>
       </c>
@@ -1805,16 +1659,8 @@
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-      <c r="N2">
-        <f t="shared" si="0"/>
-        <v>2031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1829,10 +1675,8 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1879,16 +1723,8 @@
         <f>'Pour utilisateur'!L4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="4">
-        <f>'Pour utilisateur'!M4</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <f>'Pour utilisateur'!N4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1935,16 +1771,8 @@
         <f>'Pour utilisateur'!L5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="4">
-        <f>'Pour utilisateur'!M5</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <f>'Pour utilisateur'!N5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1991,16 +1819,8 @@
         <f>'Pour utilisateur'!L6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="4">
-        <f>'Pour utilisateur'!M6</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <f>'Pour utilisateur'!N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -2015,10 +1835,8 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
@@ -2053,14 +1871,8 @@
       <c r="L9" s="8">
         <v>0.82054017639366417</v>
       </c>
-      <c r="M9" s="8">
-        <v>0.82054017639366417</v>
-      </c>
-      <c r="N9" s="8">
-        <v>0.82054017639366417</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
@@ -2073,10 +1885,8 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -2111,14 +1921,8 @@
       <c r="L11" s="9">
         <v>2.7</v>
       </c>
-      <c r="M11" s="9">
-        <v>2.7</v>
-      </c>
-      <c r="N11" s="9">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>30</v>
       </c>
@@ -2153,14 +1957,8 @@
       <c r="L12" s="9">
         <v>3.75</v>
       </c>
-      <c r="M12" s="9">
-        <v>3.75</v>
-      </c>
-      <c r="N12" s="9">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>31</v>
       </c>
@@ -2170,7 +1968,7 @@
         <v>2.134233678471138</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" ref="D13:N13" si="1">D12*D9+D11*(1-D9)</f>
+        <f t="shared" ref="D13:L13" si="1">D12*D9+D11*(1-D9)</f>
         <v>3.2006806867549988</v>
       </c>
       <c r="E13" s="9">
@@ -2205,16 +2003,8 @@
         <f t="shared" si="1"/>
         <v>3.5615671852133475</v>
       </c>
-      <c r="M13" s="9">
-        <f t="shared" si="1"/>
-        <v>3.5615671852133475</v>
-      </c>
-      <c r="N13" s="9">
-        <f t="shared" si="1"/>
-        <v>3.5615671852133475</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2227,10 +2017,8 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2243,10 +2031,8 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
@@ -2256,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <f t="shared" ref="D16:N16" si="2">(D13/100)*D6</f>
+        <f t="shared" ref="D16:L16" si="2">(D13/100)*D6</f>
         <v>0</v>
       </c>
       <c r="E16" s="10">
@@ -2291,16 +2077,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>39</v>
       </c>
@@ -2310,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" ref="D17:N17" si="3">-(D6+D16)</f>
+        <f t="shared" ref="D17:L17" si="3">-(D6+D16)</f>
         <v>0</v>
       </c>
       <c r="E17" s="10">
@@ -2345,16 +2123,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M17" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>38</v>
       </c>
@@ -2368,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="12">
-        <f t="shared" ref="E18:N18" si="4">(1+E13/100)*D18+E17</f>
+        <f t="shared" ref="E18:L18" si="4">(1+E13/100)*D18+E17</f>
         <v>0</v>
       </c>
       <c r="F18" s="12">
@@ -2399,16 +2169,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M18" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -2423,10 +2185,8 @@
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>33</v>
       </c>
@@ -2440,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" ref="E21:N21" si="5">E16+E13/100*D22</f>
+        <f t="shared" ref="E21:L21" si="5">E16+E13/100*D22</f>
         <v>0</v>
       </c>
       <c r="F21" s="16">
@@ -2471,16 +2231,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M21" s="16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>19</v>
       </c>
@@ -2490,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="16">
-        <f t="shared" ref="D22:N22" si="6">-D18</f>
+        <f t="shared" ref="D22:L22" si="6">-D18</f>
         <v>0</v>
       </c>
       <c r="E22" s="16">
@@ -2522,14 +2274,6 @@
         <v>0</v>
       </c>
       <c r="L22" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2541,9 +2285,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB77E90E-259F-4B12-BB0C-68506FD8C7E4}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2551,7 +2297,7 @@
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2563,7 +2309,7 @@
         <v>2020</v>
       </c>
       <c r="E1">
-        <f t="shared" ref="E1:N2" si="0">D1+1</f>
+        <f t="shared" ref="E1:L2" si="0">D1+1</f>
         <v>2021</v>
       </c>
       <c r="F1">
@@ -2594,16 +2340,8 @@
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="M1">
-        <f t="shared" si="0"/>
-        <v>2029</v>
-      </c>
-      <c r="N1">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2020</v>
       </c>
@@ -2643,16 +2381,8 @@
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="M2">
-        <f t="shared" si="0"/>
-        <v>2030</v>
-      </c>
-      <c r="N2">
-        <f t="shared" si="0"/>
-        <v>2031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2667,10 +2397,8 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2717,16 +2445,8 @@
         <f>'For user (EN)'!L4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="4">
-        <f>'For user (EN)'!M4</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="4">
-        <f>'For user (EN)'!N4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2773,16 +2493,8 @@
         <f>'For user (EN)'!L5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="4">
-        <f>'For user (EN)'!M5</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="4">
-        <f>'For user (EN)'!N5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -2829,16 +2541,8 @@
         <f>'For user (EN)'!L6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="4">
-        <f>'For user (EN)'!M6</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="4">
-        <f>'For user (EN)'!N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -2853,10 +2557,8 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -2891,14 +2593,8 @@
       <c r="L9" s="8">
         <v>0.82054017639366417</v>
       </c>
-      <c r="M9" s="8">
-        <v>0.82054017639366417</v>
-      </c>
-      <c r="N9" s="8">
-        <v>0.82054017639366417</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
@@ -2911,10 +2607,8 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2949,14 +2643,8 @@
       <c r="L11" s="9">
         <v>2.7</v>
       </c>
-      <c r="M11" s="9">
-        <v>2.7</v>
-      </c>
-      <c r="N11" s="9">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2991,14 +2679,8 @@
       <c r="L12" s="9">
         <v>3.75</v>
       </c>
-      <c r="M12" s="9">
-        <v>3.75</v>
-      </c>
-      <c r="N12" s="9">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -3008,7 +2690,7 @@
         <v>2.134233678471138</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" ref="D13:N13" si="1">D12*D9+D11*(1-D9)</f>
+        <f t="shared" ref="D13:L13" si="1">D12*D9+D11*(1-D9)</f>
         <v>3.2006806867549988</v>
       </c>
       <c r="E13" s="9">
@@ -3043,16 +2725,8 @@
         <f t="shared" si="1"/>
         <v>3.5615671852133475</v>
       </c>
-      <c r="M13" s="9">
-        <f t="shared" si="1"/>
-        <v>3.5615671852133475</v>
-      </c>
-      <c r="N13" s="9">
-        <f t="shared" si="1"/>
-        <v>3.5615671852133475</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3065,10 +2739,8 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3081,10 +2753,8 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
@@ -3094,7 +2764,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <f t="shared" ref="D16:N16" si="2">(D13/100)*D6</f>
+        <f t="shared" ref="D16:L16" si="2">(D13/100)*D6</f>
         <v>0</v>
       </c>
       <c r="E16" s="10">
@@ -3129,16 +2799,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>36</v>
       </c>
@@ -3148,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" ref="D17:N17" si="3">-(D6+D16)</f>
+        <f t="shared" ref="D17:L17" si="3">-(D6+D16)</f>
         <v>0</v>
       </c>
       <c r="E17" s="10">
@@ -3183,16 +2845,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M17" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>37</v>
       </c>
@@ -3206,7 +2860,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="12">
-        <f t="shared" ref="E18:N18" si="4">(1+E13/100)*D18+E17</f>
+        <f t="shared" ref="E18:L18" si="4">(1+E13/100)*D18+E17</f>
         <v>0</v>
       </c>
       <c r="F18" s="12">
@@ -3237,16 +2891,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M18" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -3261,10 +2907,8 @@
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>12</v>
       </c>
@@ -3278,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" ref="E21:N21" si="5">E16+E13/100*D22</f>
+        <f t="shared" ref="E21:L21" si="5">E16+E13/100*D22</f>
         <v>0</v>
       </c>
       <c r="F21" s="16">
@@ -3309,16 +2953,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M21" s="16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>13</v>
       </c>
@@ -3328,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="16">
-        <f t="shared" ref="D22:N22" si="6">-D18</f>
+        <f t="shared" ref="D22:L22" si="6">-D18</f>
         <v>0</v>
       </c>
       <c r="E22" s="16">
@@ -3363,16 +2999,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M22" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -3383,10 +3011,8 @@
       <c r="J25" s="21"/>
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C26" s="23"/>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -3397,10 +3023,8 @@
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C27" s="22"/>
     </row>
   </sheetData>

</xml_diff>